<commit_message>
update lib and examples
</commit_message>
<xml_diff>
--- a/STM32/libraries/BoardExamples/examples/all_boards/Benchmarks/Benchmarks-results.xlsx
+++ b/STM32/libraries/BoardExamples/examples/all_boards/Benchmarks/Benchmarks-results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="18225" windowHeight="10125"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Board</t>
   </si>
@@ -231,6 +231,10 @@
   </si>
   <si>
     <t>EFM32G222F</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NANO120</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -941,22 +945,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1303,13 +1307,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
+      <selection pane="bottomRight" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1337,16 +1341,17 @@
     <col min="22" max="22" width="7.375" customWidth="1"/>
     <col min="23" max="23" width="8.125" customWidth="1"/>
     <col min="24" max="24" width="7.5" customWidth="1"/>
+    <col min="25" max="25" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="17" t="s">
         <v>51</v>
       </c>
@@ -1371,27 +1376,30 @@
         <v>52</v>
       </c>
       <c r="O1" s="18"/>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="16"/>
+      <c r="Q1" s="20"/>
       <c r="R1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="15" t="s">
+      <c r="T1" s="20"/>
+      <c r="U1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="V1" s="16"/>
+      <c r="V1" s="20"/>
       <c r="W1" s="17" t="s">
         <v>61</v>
       </c>
       <c r="X1" s="21"/>
-    </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>36</v>
       </c>
@@ -1464,8 +1472,11 @@
       <c r="X2" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y2" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>35</v>
       </c>
@@ -1538,8 +1549,11 @@
       <c r="X3" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>58</v>
@@ -1576,8 +1590,9 @@
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -1644,8 +1659,9 @@
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -1714,8 +1730,11 @@
       <c r="X6" s="12">
         <v>25764</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y6" s="12">
+        <v>36208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
@@ -1786,8 +1805,11 @@
       <c r="X7" s="3">
         <v>14.66</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y7" s="3">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1812,8 +1834,9 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y8" s="3"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
@@ -1872,8 +1895,9 @@
       </c>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y9" s="12"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -1932,8 +1956,9 @@
       </c>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y10" s="12"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
@@ -1960,23 +1985,24 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C16" s="6" t="s">
         <v>48</v>
       </c>

</xml_diff>